<commit_message>
LapNV: Update Create Trip
</commit_message>
<xml_diff>
--- a/References/ReqDocs/Driver/03_Home.xlsx
+++ b/References/ReqDocs/Driver/03_Home.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="450" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="900" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="03.Home" sheetId="1" r:id="rId1"/>
@@ -449,7 +449,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -471,6 +471,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -758,7 +764,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -818,6 +824,21 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -854,21 +875,8 @@
     <xf numFmtId="0" fontId="2" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1555,8 +1563,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A3:AS80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="Q62" sqref="Q62"/>
+    <sheetView tabSelected="1" topLeftCell="I22" workbookViewId="0">
+      <selection activeCell="X43" sqref="X43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1575,10 +1583,10 @@
       <c r="C4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D4" s="65" t="s">
+      <c r="D4" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="65"/>
+      <c r="E4" s="55"/>
       <c r="F4" s="2" t="s">
         <v>2</v>
       </c>
@@ -1586,30 +1594,30 @@
       <c r="J4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="K4" s="65" t="s">
+      <c r="K4" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="L4" s="65"/>
+      <c r="L4" s="55"/>
       <c r="M4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="P4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="Q4" s="65" t="s">
+      <c r="Q4" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="R4" s="65"/>
+      <c r="R4" s="55"/>
       <c r="S4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="V4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="W4" s="65" t="s">
+      <c r="W4" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="X4" s="65"/>
+      <c r="X4" s="55"/>
       <c r="Y4" s="2" t="s">
         <v>2</v>
       </c>
@@ -1733,18 +1741,18 @@
       <c r="W10" s="5"/>
       <c r="X10" s="5"/>
       <c r="Y10" s="6"/>
-      <c r="AB10" s="66" t="s">
+      <c r="AB10" s="56" t="s">
         <v>5</v>
       </c>
-      <c r="AC10" s="66"/>
-      <c r="AD10" s="66"/>
-      <c r="AE10" s="66"/>
-      <c r="AG10" s="68" t="s">
+      <c r="AC10" s="56"/>
+      <c r="AD10" s="56"/>
+      <c r="AE10" s="56"/>
+      <c r="AG10" s="53" t="s">
         <v>6</v>
       </c>
-      <c r="AH10" s="68"/>
-      <c r="AI10" s="68"/>
-      <c r="AJ10" s="68"/>
+      <c r="AH10" s="53"/>
+      <c r="AI10" s="53"/>
+      <c r="AJ10" s="53"/>
     </row>
     <row r="11" spans="3:36" x14ac:dyDescent="0.25">
       <c r="C11" s="4"/>
@@ -1759,14 +1767,14 @@
       <c r="V11" s="4"/>
       <c r="X11" s="5"/>
       <c r="Y11" s="6"/>
-      <c r="AB11" s="66"/>
-      <c r="AC11" s="66"/>
-      <c r="AD11" s="66"/>
-      <c r="AE11" s="66"/>
-      <c r="AG11" s="68"/>
-      <c r="AH11" s="68"/>
-      <c r="AI11" s="68"/>
-      <c r="AJ11" s="68"/>
+      <c r="AB11" s="56"/>
+      <c r="AC11" s="56"/>
+      <c r="AD11" s="56"/>
+      <c r="AE11" s="56"/>
+      <c r="AG11" s="53"/>
+      <c r="AH11" s="53"/>
+      <c r="AI11" s="53"/>
+      <c r="AJ11" s="53"/>
     </row>
     <row r="12" spans="3:36" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="4"/>
@@ -1785,14 +1793,14 @@
       <c r="W12" s="5"/>
       <c r="X12" s="5"/>
       <c r="Y12" s="6"/>
-      <c r="AB12" s="67"/>
-      <c r="AC12" s="67"/>
-      <c r="AD12" s="67"/>
-      <c r="AE12" s="67"/>
-      <c r="AG12" s="69"/>
-      <c r="AH12" s="69"/>
-      <c r="AI12" s="69"/>
-      <c r="AJ12" s="69"/>
+      <c r="AB12" s="57"/>
+      <c r="AC12" s="57"/>
+      <c r="AD12" s="57"/>
+      <c r="AE12" s="57"/>
+      <c r="AG12" s="54"/>
+      <c r="AH12" s="54"/>
+      <c r="AI12" s="54"/>
+      <c r="AJ12" s="54"/>
     </row>
     <row r="13" spans="3:36" x14ac:dyDescent="0.25">
       <c r="C13" s="4"/>
@@ -1820,16 +1828,16 @@
       </c>
       <c r="Y13" s="6"/>
       <c r="AB13" s="8"/>
-      <c r="AC13" s="56" t="s">
+      <c r="AC13" s="61" t="s">
         <v>8</v>
       </c>
-      <c r="AD13" s="56"/>
+      <c r="AD13" s="61"/>
       <c r="AE13" s="9"/>
       <c r="AG13" s="8"/>
-      <c r="AH13" s="56" t="s">
+      <c r="AH13" s="61" t="s">
         <v>8</v>
       </c>
-      <c r="AI13" s="56"/>
+      <c r="AI13" s="61"/>
       <c r="AJ13" s="9"/>
     </row>
     <row r="14" spans="3:36" x14ac:dyDescent="0.25">
@@ -1877,18 +1885,18 @@
       <c r="W15" s="5"/>
       <c r="X15" s="5"/>
       <c r="Y15" s="6"/>
-      <c r="AB15" s="57" t="s">
+      <c r="AB15" s="62" t="s">
         <v>10</v>
       </c>
-      <c r="AC15" s="58"/>
-      <c r="AD15" s="58"/>
-      <c r="AE15" s="59"/>
-      <c r="AG15" s="57" t="s">
+      <c r="AC15" s="63"/>
+      <c r="AD15" s="63"/>
+      <c r="AE15" s="64"/>
+      <c r="AG15" s="62" t="s">
         <v>11</v>
       </c>
-      <c r="AH15" s="58"/>
-      <c r="AI15" s="58"/>
-      <c r="AJ15" s="59"/>
+      <c r="AH15" s="63"/>
+      <c r="AI15" s="63"/>
+      <c r="AJ15" s="64"/>
     </row>
     <row r="16" spans="3:36" x14ac:dyDescent="0.25">
       <c r="C16" s="4"/>
@@ -1911,14 +1919,14 @@
       <c r="W16" s="5"/>
       <c r="X16" s="5"/>
       <c r="Y16" s="6"/>
-      <c r="AB16" s="57"/>
-      <c r="AC16" s="58"/>
-      <c r="AD16" s="58"/>
-      <c r="AE16" s="59"/>
-      <c r="AG16" s="57"/>
-      <c r="AH16" s="58"/>
-      <c r="AI16" s="58"/>
-      <c r="AJ16" s="59"/>
+      <c r="AB16" s="62"/>
+      <c r="AC16" s="63"/>
+      <c r="AD16" s="63"/>
+      <c r="AE16" s="64"/>
+      <c r="AG16" s="62"/>
+      <c r="AH16" s="63"/>
+      <c r="AI16" s="63"/>
+      <c r="AJ16" s="64"/>
     </row>
     <row r="17" spans="1:45" x14ac:dyDescent="0.25">
       <c r="C17" s="4"/>
@@ -2031,7 +2039,7 @@
       <c r="AJ19" s="6"/>
     </row>
     <row r="20" spans="1:45" x14ac:dyDescent="0.25">
-      <c r="C20" s="60" t="s">
+      <c r="C20" s="65" t="s">
         <v>25</v>
       </c>
       <c r="D20" s="12" t="s">
@@ -2039,7 +2047,7 @@
       </c>
       <c r="E20" s="13"/>
       <c r="F20" s="14"/>
-      <c r="J20" s="60" t="s">
+      <c r="J20" s="65" t="s">
         <v>25</v>
       </c>
       <c r="K20" s="12" t="s">
@@ -2047,7 +2055,7 @@
       </c>
       <c r="L20" s="13"/>
       <c r="M20" s="14"/>
-      <c r="P20" s="60"/>
+      <c r="P20" s="65"/>
       <c r="Q20" s="13"/>
       <c r="R20" s="13"/>
       <c r="S20" s="14"/>
@@ -2065,7 +2073,7 @@
       <c r="AJ20" s="6"/>
     </row>
     <row r="21" spans="1:45" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C21" s="61"/>
+      <c r="C21" s="66"/>
       <c r="D21" s="20" t="s">
         <v>27</v>
       </c>
@@ -2073,7 +2081,7 @@
       <c r="F21" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="J21" s="61"/>
+      <c r="J21" s="66"/>
       <c r="K21" s="20" t="s">
         <v>29</v>
       </c>
@@ -2081,18 +2089,18 @@
       <c r="M21" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="P21" s="61"/>
+      <c r="P21" s="66"/>
       <c r="Q21" s="20" t="s">
         <v>31</v>
       </c>
       <c r="R21" s="20"/>
       <c r="S21" s="21"/>
-      <c r="V21" s="62" t="s">
+      <c r="V21" s="67" t="s">
         <v>32</v>
       </c>
-      <c r="W21" s="63"/>
-      <c r="X21" s="63"/>
-      <c r="Y21" s="64"/>
+      <c r="W21" s="68"/>
+      <c r="X21" s="68"/>
+      <c r="Y21" s="69"/>
       <c r="AB21" s="22"/>
       <c r="AC21" s="23"/>
       <c r="AD21" s="23"/>
@@ -2734,16 +2742,16 @@
       <c r="J41" s="5"/>
       <c r="K41" s="5"/>
       <c r="L41" s="5"/>
-      <c r="M41" s="5"/>
-      <c r="N41" s="5"/>
-      <c r="O41" s="5"/>
-      <c r="P41" s="5"/>
-      <c r="Q41" s="5"/>
-      <c r="R41" s="5"/>
-      <c r="S41" s="41"/>
-      <c r="T41" s="5"/>
-      <c r="U41" s="41"/>
-      <c r="V41" s="41"/>
+      <c r="M41" s="70"/>
+      <c r="N41" s="70"/>
+      <c r="O41" s="70"/>
+      <c r="P41" s="70"/>
+      <c r="Q41" s="70"/>
+      <c r="R41" s="70"/>
+      <c r="S41" s="71"/>
+      <c r="T41" s="70"/>
+      <c r="U41" s="71"/>
+      <c r="V41" s="71"/>
       <c r="W41" s="41"/>
       <c r="X41" s="41"/>
       <c r="Y41" s="41"/>
@@ -2926,51 +2934,51 @@
       <c r="B45" s="34">
         <v>14</v>
       </c>
-      <c r="C45" s="53" t="s">
+      <c r="C45" s="58" t="s">
         <v>57</v>
       </c>
-      <c r="D45" s="54"/>
-      <c r="E45" s="54"/>
-      <c r="F45" s="54"/>
-      <c r="G45" s="54"/>
-      <c r="H45" s="54"/>
-      <c r="I45" s="54"/>
-      <c r="J45" s="54"/>
-      <c r="K45" s="54"/>
-      <c r="L45" s="54"/>
-      <c r="M45" s="54"/>
-      <c r="N45" s="54"/>
-      <c r="O45" s="54"/>
-      <c r="P45" s="54"/>
-      <c r="Q45" s="54"/>
-      <c r="R45" s="54"/>
-      <c r="S45" s="54"/>
-      <c r="T45" s="54"/>
-      <c r="U45" s="54"/>
-      <c r="V45" s="54"/>
-      <c r="W45" s="54"/>
-      <c r="X45" s="54"/>
-      <c r="Y45" s="54"/>
-      <c r="Z45" s="54"/>
-      <c r="AA45" s="54"/>
-      <c r="AB45" s="54"/>
-      <c r="AC45" s="54"/>
-      <c r="AD45" s="54"/>
-      <c r="AE45" s="54"/>
-      <c r="AF45" s="54"/>
-      <c r="AG45" s="54"/>
-      <c r="AH45" s="54"/>
-      <c r="AI45" s="54"/>
-      <c r="AJ45" s="54"/>
-      <c r="AK45" s="54"/>
-      <c r="AL45" s="54"/>
-      <c r="AM45" s="54"/>
-      <c r="AN45" s="54"/>
-      <c r="AO45" s="54"/>
-      <c r="AP45" s="54"/>
-      <c r="AQ45" s="54"/>
-      <c r="AR45" s="54"/>
-      <c r="AS45" s="55"/>
+      <c r="D45" s="59"/>
+      <c r="E45" s="59"/>
+      <c r="F45" s="59"/>
+      <c r="G45" s="59"/>
+      <c r="H45" s="59"/>
+      <c r="I45" s="59"/>
+      <c r="J45" s="59"/>
+      <c r="K45" s="59"/>
+      <c r="L45" s="59"/>
+      <c r="M45" s="59"/>
+      <c r="N45" s="59"/>
+      <c r="O45" s="59"/>
+      <c r="P45" s="59"/>
+      <c r="Q45" s="59"/>
+      <c r="R45" s="59"/>
+      <c r="S45" s="59"/>
+      <c r="T45" s="59"/>
+      <c r="U45" s="59"/>
+      <c r="V45" s="59"/>
+      <c r="W45" s="59"/>
+      <c r="X45" s="59"/>
+      <c r="Y45" s="59"/>
+      <c r="Z45" s="59"/>
+      <c r="AA45" s="59"/>
+      <c r="AB45" s="59"/>
+      <c r="AC45" s="59"/>
+      <c r="AD45" s="59"/>
+      <c r="AE45" s="59"/>
+      <c r="AF45" s="59"/>
+      <c r="AG45" s="59"/>
+      <c r="AH45" s="59"/>
+      <c r="AI45" s="59"/>
+      <c r="AJ45" s="59"/>
+      <c r="AK45" s="59"/>
+      <c r="AL45" s="59"/>
+      <c r="AM45" s="59"/>
+      <c r="AN45" s="59"/>
+      <c r="AO45" s="59"/>
+      <c r="AP45" s="59"/>
+      <c r="AQ45" s="59"/>
+      <c r="AR45" s="59"/>
+      <c r="AS45" s="60"/>
     </row>
     <row r="46" spans="1:45" s="29" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="26"/>
@@ -3131,12 +3139,6 @@
     </row>
   </sheetData>
   <mergeCells count="15">
-    <mergeCell ref="AG10:AJ12"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="Q4:R4"/>
-    <mergeCell ref="W4:X4"/>
-    <mergeCell ref="AB10:AE12"/>
     <mergeCell ref="C45:AS45"/>
     <mergeCell ref="AC13:AD13"/>
     <mergeCell ref="AH13:AI13"/>
@@ -3146,6 +3148,12 @@
     <mergeCell ref="J20:J21"/>
     <mergeCell ref="P20:P21"/>
     <mergeCell ref="V21:Y21"/>
+    <mergeCell ref="AG10:AJ12"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="Q4:R4"/>
+    <mergeCell ref="W4:X4"/>
+    <mergeCell ref="AB10:AE12"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>